<commit_message>
Mejora a la interfaz para distintas resoluciones, cambio a nombre de campos en modo aqua, se agregan campos de Impuestos sobre la renta y descuentos por seguro social y seguro educativo
</commit_message>
<xml_diff>
--- a/nomina_quincenal_pago_20251215.xlsx
+++ b/nomina_quincenal_pago_20251215.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,70 +466,95 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Empleado por contrato</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Salario Base</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Quincena Inicio</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Quincena Fin</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Fecha de Pago</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Total Horas Trabajadas</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Horas Extra (después 3 PM)</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Pago Extra (25% adicional)</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Bono Horas Extra</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Horas Feriado/Domingo</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Pago Feriado/Domingo (50% adicional)</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Seguro Social (3%)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Seguro Educativo (5%)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ISL</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Total Descuentos</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Número de Cuenta</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Banco</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Tipo de Cuenta</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Total Pago a Empleados</t>
         </is>
@@ -566,58 +591,75 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
         <v>5.98</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>99</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>1</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>7.48</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>86.04000000000001</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>0-465972284592</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="Y2" t="n">
         <v>593.52</v>
       </c>
     </row>
@@ -652,58 +694,75 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
         <v>5.98</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>95.5</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
         <v>71.09</v>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
       <c r="P3" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="inlineStr">
         <is>
           <t>0-441988638943</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="X3" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="T3" t="n">
+      <c r="Y3" t="n">
         <v>571.09</v>
       </c>
     </row>
@@ -738,30 +797,32 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
         <v>4.41</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>98</v>
       </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
@@ -774,22 +835,37 @@
       <c r="P4" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="inlineStr">
         <is>
           <t>0-419972553348</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="W4" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="X4" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="T4" t="n">
+      <c r="Y4" t="n">
         <v>432.18</v>
       </c>
     </row>
@@ -824,30 +900,32 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
         <v>4.41</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>98</v>
       </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
@@ -860,22 +938,37 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>0-441966573634</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="W5" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="X5" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="T5" t="n">
+      <c r="Y5" t="n">
         <v>432.18</v>
       </c>
     </row>
@@ -910,58 +1003,75 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
         <v>5.98</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>98</v>
       </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
         <v>86.04000000000001</v>
       </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr">
         <is>
           <t>0-465960167120</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="W6" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="X6" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="T6" t="n">
+      <c r="Y6" t="n">
         <v>586.04</v>
       </c>
     </row>
@@ -996,30 +1106,32 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
         <v>5</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>98</v>
       </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
@@ -1032,22 +1144,37 @@
       <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="inlineStr">
         <is>
           <t>0-465984269473</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="W7" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="X7" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="T7" t="n">
+      <c r="Y7" t="n">
         <v>490</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejora a la resolucion, se agrega opcion de prestamos a empleados, mejoramiento de GUI
</commit_message>
<xml_diff>
--- a/nomina_quincenal_pago_20251215.xlsx
+++ b/nomina_quincenal_pago_20251215.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,12 +521,12 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Seguro Social (3%)</t>
+          <t>Seguro Social (9.75%)</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Seguro Educativo (5%)</t>
+          <t>Seguro Educativo (1.25%)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
@@ -536,25 +536,35 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>Descuento Préstamo</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>Total Descuentos</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Total Saldo Préstamo</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Número de Cuenta</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Banco</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Tipo de Cuenta</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Total Pago a Empleados</t>
         </is>
@@ -644,22 +654,28 @@
       <c r="U2" t="n">
         <v>0</v>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="inlineStr">
         <is>
           <t>0-465972284592</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="Y2" t="n">
+      <c r="AA2" t="n">
         <v>593.52</v>
       </c>
     </row>
@@ -747,22 +763,28 @@
       <c r="U3" t="n">
         <v>0</v>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>0-441988638943</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="Y3" t="n">
+      <c r="AA3" t="n">
         <v>571.09</v>
       </c>
     </row>
@@ -850,22 +872,28 @@
       <c r="U4" t="n">
         <v>0</v>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="inlineStr">
         <is>
           <t>0-419972553348</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="Y4" t="n">
+      <c r="AA4" t="n">
         <v>432.18</v>
       </c>
     </row>
@@ -953,22 +981,28 @@
       <c r="U5" t="n">
         <v>0</v>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>40</v>
+      </c>
+      <c r="X5" t="inlineStr">
         <is>
           <t>0-441966573634</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="X5" t="inlineStr">
+      <c r="Z5" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="Y5" t="n">
+      <c r="AA5" t="n">
         <v>432.18</v>
       </c>
     </row>
@@ -1056,22 +1090,28 @@
       <c r="U6" t="n">
         <v>0</v>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="inlineStr">
         <is>
           <t>0-465960167120</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
+      <c r="Y6" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="Y6" t="n">
+      <c r="AA6" t="n">
         <v>586.04</v>
       </c>
     </row>
@@ -1159,22 +1199,28 @@
       <c r="U7" t="n">
         <v>0</v>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="inlineStr">
         <is>
           <t>0-465984269473</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="X7" t="inlineStr">
+      <c r="Z7" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="Y7" t="n">
+      <c r="AA7" t="n">
         <v>490</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se mejoran botones de pagina principal, se agrega calculo de nomina para empleados de seguridad y se mejora la seleccion de empleados a la hora de eliminarlos
</commit_message>
<xml_diff>
--- a/nomina_quincenal_pago_20251215.xlsx
+++ b/nomina_quincenal_pago_20251215.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,105 +466,170 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Seguridad</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Empleado por contrato</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Salario Base</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Quincena Inicio</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Quincena Fin</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Fecha de Pago</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Total Horas Trabajadas</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Horas Extra (después 3 PM)</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Pago Extra (25% adicional)</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Bono Horas Extra</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Horas Feriado/Domingo</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Pago Feriado/Domingo (50% adicional)</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Horas Turno Seguridad</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Hora Cambio Turno Seguridad</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Margen Salida Seguridad (min)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Tolerancia Turno Seguridad (min)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Horas Reales Seguridad (prom)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Dif Turno Seguridad (min, prom)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Alerta Seguridad</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Turnos Seguridad Día</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Turnos Seguridad Noche</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Total Turnos Seguridad</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Empleados Seguridad Turno Día</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Empleados Seguridad Turno Noche</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Seguro Social (9.75%)</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Seguro Educativo (1.25%)</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>ISL</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Descuento Préstamo</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Total Descuentos</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Total Saldo Préstamo</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Número de Cuenta</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Banco</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Tipo de Cuenta</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Total Pago a Empleados</t>
         </is>
@@ -606,76 +671,93 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
         <v>5.98</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>99</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>7.48</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>86.04000000000001</v>
       </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="inlineStr">
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>0-465972284592</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="AA2" t="n">
+      <c r="AN2" t="n">
         <v>593.52</v>
       </c>
     </row>
@@ -715,76 +797,93 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
         <v>5.98</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>95.5</v>
       </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
         <v>71.09</v>
       </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="inlineStr">
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>0-441988638943</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="AL3" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="AM3" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="AA3" t="n">
+      <c r="AN3" t="n">
         <v>571.09</v>
       </c>
     </row>
@@ -824,30 +923,32 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
         <v>4.41</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>98</v>
       </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
       <c r="N4" t="n">
         <v>0</v>
       </c>
@@ -863,37 +964,52 @@
       <c r="R4" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" t="inlineStr">
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="inlineStr">
         <is>
           <t>0-419972553348</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="AL4" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="Z4" t="inlineStr">
+      <c r="AM4" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="AA4" t="n">
+      <c r="AN4" t="n">
         <v>432.18</v>
       </c>
     </row>
@@ -933,30 +1049,32 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
         <v>4.41</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>98</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
@@ -972,37 +1090,52 @@
       <c r="R5" t="n">
         <v>0</v>
       </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="n">
-        <v>40</v>
-      </c>
-      <c r="X5" t="inlineStr">
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AK5" t="inlineStr">
         <is>
           <t>0-441966573634</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr">
+      <c r="AL5" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr">
+      <c r="AM5" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="AA5" t="n">
+      <c r="AN5" t="n">
         <v>432.18</v>
       </c>
     </row>
@@ -1042,76 +1175,93 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
         <v>5.98</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>98</v>
       </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
         <v>86.04000000000001</v>
       </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" t="inlineStr">
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="inlineStr">
         <is>
           <t>0-465960167120</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="AL6" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr">
+      <c r="AM6" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="AA6" t="n">
+      <c r="AN6" t="n">
         <v>586.04</v>
       </c>
     </row>
@@ -1151,30 +1301,32 @@
           <t>No</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
         <v>5</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>15/12/2025</t>
         </is>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>98</v>
       </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
@@ -1190,37 +1342,52 @@
       <c r="R7" t="n">
         <v>0</v>
       </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" t="inlineStr">
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="inlineStr">
         <is>
           <t>0-465984269473</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
+      <c r="AL7" t="inlineStr">
         <is>
           <t>Banco General</t>
         </is>
       </c>
-      <c r="Z7" t="inlineStr">
+      <c r="AM7" t="inlineStr">
         <is>
           <t>Ahorro</t>
         </is>
       </c>
-      <c r="AA7" t="n">
+      <c r="AN7" t="n">
         <v>490</v>
       </c>
     </row>

</xml_diff>